<commit_message>
listados del 12 de agosto de 2024
</commit_message>
<xml_diff>
--- a/Agosto/12 agosto/iguala/LISTA DE ASPIRANTES_ITIGUALA 2024-2.xlsx
+++ b/Agosto/12 agosto/iguala/LISTA DE ASPIRANTES_ITIGUALA 2024-2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proyecto01TICs\Documents\Evaluatec2024\Agosto\12 agosto\iguala\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxoC\OneDrive\Documents\EVALUATEC2024\Agosto\12 agosto\iguala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9817214B-5E41-44D3-8708-6ECE0B4B2700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF477D1-EAA6-40A8-8F14-0947988A8835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1060,6 +1060,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1069,7 +1070,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Encabezado 1" xfId="1" builtinId="16"/>
@@ -1125,13 +1125,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A4:M97" totalsRowShown="0">
-  <autoFilter ref="A4:M97" xr:uid="{00000000-0009-0000-0100-000002000000}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="CONTADOR PUBLICO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A4:M97" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:M97">
     <sortCondition ref="E4:E97"/>
   </sortState>
@@ -1453,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1475,28 +1469,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="15" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="L2" s="17"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="L3" s="17"/>
+      <c r="L3" s="18"/>
     </row>
     <row r="4" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1616,8 +1610,8 @@
         <v>23</v>
       </c>
       <c r="M6" s="3"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
     </row>
     <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -2321,7 +2315,7 @@
       </c>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2501</v>
       </c>
@@ -2360,7 +2354,7 @@
       </c>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2499</v>
       </c>
@@ -2399,7 +2393,7 @@
       </c>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2486</v>
       </c>
@@ -2438,7 +2432,7 @@
       </c>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2472</v>
       </c>
@@ -2477,7 +2471,7 @@
       </c>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2467</v>
       </c>
@@ -2516,7 +2510,7 @@
       </c>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2461</v>
       </c>
@@ -2555,7 +2549,7 @@
       </c>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2384</v>
       </c>
@@ -2594,7 +2588,7 @@
       </c>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2363</v>
       </c>
@@ -2633,7 +2627,7 @@
       </c>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2350</v>
       </c>
@@ -2672,7 +2666,7 @@
       </c>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2347</v>
       </c>
@@ -2711,7 +2705,7 @@
       </c>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2313</v>
       </c>
@@ -2750,7 +2744,7 @@
       </c>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2924</v>
       </c>
@@ -2789,7 +2783,7 @@
       </c>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2917</v>
       </c>
@@ -2828,7 +2822,7 @@
       </c>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2916</v>
       </c>
@@ -2867,7 +2861,7 @@
       </c>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2915</v>
       </c>
@@ -2906,7 +2900,7 @@
       </c>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2899</v>
       </c>
@@ -2945,7 +2939,7 @@
       </c>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2898</v>
       </c>
@@ -2984,7 +2978,7 @@
       </c>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" ht="45.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2897</v>
       </c>
@@ -3023,7 +3017,7 @@
       </c>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" ht="36.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2895</v>
       </c>
@@ -3062,7 +3056,7 @@
       </c>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2894</v>
       </c>
@@ -3101,7 +3095,7 @@
       </c>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" ht="42.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2878</v>
       </c>
@@ -3140,7 +3134,7 @@
       </c>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" ht="41.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2877</v>
       </c>
@@ -3179,7 +3173,7 @@
       </c>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13" ht="43.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2871</v>
       </c>
@@ -3218,7 +3212,7 @@
       </c>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2866</v>
       </c>
@@ -3257,7 +3251,7 @@
       </c>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" ht="41.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2861</v>
       </c>
@@ -3296,7 +3290,7 @@
       </c>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2496</v>
       </c>
@@ -3335,7 +3329,7 @@
       </c>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2481</v>
       </c>
@@ -3374,7 +3368,7 @@
       </c>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2387</v>
       </c>
@@ -3413,7 +3407,7 @@
       </c>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2380</v>
       </c>
@@ -3452,7 +3446,7 @@
       </c>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2296</v>
       </c>
@@ -3491,7 +3485,7 @@
       </c>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2931</v>
       </c>
@@ -3530,7 +3524,7 @@
       </c>
       <c r="M55" s="3"/>
     </row>
-    <row r="56" spans="1:13" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2926</v>
       </c>
@@ -3569,7 +3563,7 @@
       </c>
       <c r="M56" s="3"/>
     </row>
-    <row r="57" spans="1:13" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2920</v>
       </c>
@@ -3608,7 +3602,7 @@
       </c>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2919</v>
       </c>
@@ -3647,7 +3641,7 @@
       </c>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="1:13" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2914</v>
       </c>
@@ -3686,7 +3680,7 @@
       </c>
       <c r="M59" s="3"/>
     </row>
-    <row r="60" spans="1:13" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2913</v>
       </c>
@@ -3725,7 +3719,7 @@
       </c>
       <c r="M60" s="3"/>
     </row>
-    <row r="61" spans="1:13" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2906</v>
       </c>
@@ -3764,7 +3758,7 @@
       </c>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2905</v>
       </c>
@@ -3803,7 +3797,7 @@
       </c>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2903</v>
       </c>
@@ -3842,7 +3836,7 @@
       </c>
       <c r="M63" s="3"/>
     </row>
-    <row r="64" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2891</v>
       </c>
@@ -3881,7 +3875,7 @@
       </c>
       <c r="M64" s="3"/>
     </row>
-    <row r="65" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2881</v>
       </c>
@@ -3920,7 +3914,7 @@
       </c>
       <c r="M65" s="3"/>
     </row>
-    <row r="66" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2875</v>
       </c>
@@ -3959,7 +3953,7 @@
       </c>
       <c r="M66" s="3"/>
     </row>
-    <row r="67" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2873</v>
       </c>
@@ -3998,7 +3992,7 @@
       </c>
       <c r="M67" s="3"/>
     </row>
-    <row r="68" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2869</v>
       </c>
@@ -4037,7 +4031,7 @@
       </c>
       <c r="M68" s="3"/>
     </row>
-    <row r="69" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2862</v>
       </c>
@@ -4076,7 +4070,7 @@
       </c>
       <c r="M69" s="3"/>
     </row>
-    <row r="70" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2857</v>
       </c>
@@ -4115,7 +4109,7 @@
       </c>
       <c r="M70" s="3"/>
     </row>
-    <row r="71" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2856</v>
       </c>
@@ -4154,7 +4148,7 @@
       </c>
       <c r="M71" s="3"/>
     </row>
-    <row r="72" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2500</v>
       </c>
@@ -4193,7 +4187,7 @@
       </c>
       <c r="M72" s="3"/>
     </row>
-    <row r="73" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2487</v>
       </c>
@@ -4232,7 +4226,7 @@
       </c>
       <c r="M73" s="3"/>
     </row>
-    <row r="74" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2447</v>
       </c>
@@ -4271,7 +4265,7 @@
       </c>
       <c r="M74" s="3"/>
     </row>
-    <row r="75" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2419</v>
       </c>
@@ -4310,7 +4304,7 @@
       </c>
       <c r="M75" s="3"/>
     </row>
-    <row r="76" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2414</v>
       </c>
@@ -4349,7 +4343,7 @@
       </c>
       <c r="M76" s="3"/>
     </row>
-    <row r="77" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2902</v>
       </c>
@@ -4388,7 +4382,7 @@
       </c>
       <c r="M77" s="3"/>
     </row>
-    <row r="78" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2892</v>
       </c>
@@ -4427,7 +4421,7 @@
       </c>
       <c r="M78" s="3"/>
     </row>
-    <row r="79" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2886</v>
       </c>
@@ -4466,7 +4460,7 @@
       </c>
       <c r="M79" s="3"/>
     </row>
-    <row r="80" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2879</v>
       </c>
@@ -4505,7 +4499,7 @@
       </c>
       <c r="M80" s="3"/>
     </row>
-    <row r="81" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2863</v>
       </c>
@@ -4544,7 +4538,7 @@
       </c>
       <c r="M81" s="3"/>
     </row>
-    <row r="82" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2491</v>
       </c>
@@ -4583,7 +4577,7 @@
       </c>
       <c r="M82" s="3"/>
     </row>
-    <row r="83" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2490</v>
       </c>
@@ -4622,7 +4616,7 @@
       </c>
       <c r="M83" s="3"/>
     </row>
-    <row r="84" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2482</v>
       </c>
@@ -4661,7 +4655,7 @@
       </c>
       <c r="M84" s="3"/>
     </row>
-    <row r="85" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2473</v>
       </c>
@@ -4700,7 +4694,7 @@
       </c>
       <c r="M85" s="3"/>
     </row>
-    <row r="86" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2463</v>
       </c>
@@ -4739,7 +4733,7 @@
       </c>
       <c r="M86" s="3"/>
     </row>
-    <row r="87" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2438</v>
       </c>
@@ -4778,7 +4772,7 @@
       </c>
       <c r="M87" s="3"/>
     </row>
-    <row r="88" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2434</v>
       </c>
@@ -4817,7 +4811,7 @@
       </c>
       <c r="M88" s="3"/>
     </row>
-    <row r="89" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2424</v>
       </c>
@@ -4856,7 +4850,7 @@
       </c>
       <c r="M89" s="3"/>
     </row>
-    <row r="90" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2422</v>
       </c>
@@ -4895,7 +4889,7 @@
       </c>
       <c r="M90" s="3"/>
     </row>
-    <row r="91" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2918</v>
       </c>
@@ -4934,7 +4928,7 @@
       </c>
       <c r="M91" s="3"/>
     </row>
-    <row r="92" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2912</v>
       </c>
@@ -4973,7 +4967,7 @@
       </c>
       <c r="M92" s="3"/>
     </row>
-    <row r="93" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2901</v>
       </c>
@@ -5012,7 +5006,7 @@
       </c>
       <c r="M93" s="3"/>
     </row>
-    <row r="94" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2890</v>
       </c>
@@ -5051,7 +5045,7 @@
       </c>
       <c r="M94" s="3"/>
     </row>
-    <row r="95" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2889</v>
       </c>
@@ -5090,7 +5084,7 @@
       </c>
       <c r="M95" s="3"/>
     </row>
-    <row r="96" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2868</v>
       </c>
@@ -5129,7 +5123,7 @@
       </c>
       <c r="M96" s="3"/>
     </row>
-    <row r="97" spans="5:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E97" s="1"/>
       <c r="H97" s="12"/>
       <c r="I97" s="13"/>

</xml_diff>